<commit_message>
removed double "counting" of atezo in look-up
</commit_message>
<xml_diff>
--- a/data-raw/treatment-costs.xlsx
+++ b/data-raw/treatment-costs.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW GENERAL (MANAGEMENT)/Jeroen only access/IVI/GitHub/IVI-NSCLC/data-raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724F2A24-8B3D-0E49-99C3-44809F1933E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26580" yWindow="-21600" windowWidth="36780" windowHeight="20160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18920" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dosage" sheetId="1" r:id="rId1"/>
@@ -13,7 +19,7 @@
     <sheet name="administration_costs" sheetId="3" r:id="rId4"/>
     <sheet name="lookup" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="113">
   <si>
     <t>erlotinib</t>
   </si>
@@ -367,7 +373,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -1235,6 +1241,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1559,7 +1573,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1569,7 +1583,7 @@
       <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
@@ -1583,7 +1597,7 @@
     <col min="11" max="11" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>72</v>
       </c>
@@ -1618,7 +1632,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
@@ -1684,7 +1698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
@@ -1717,7 +1731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>13</v>
       </c>
@@ -1750,7 +1764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>52</v>
       </c>
@@ -1783,7 +1797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="60">
+    <row r="7" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1820,7 +1834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
@@ -1852,7 +1866,7 @@
       </c>
       <c r="K8" s="16"/>
     </row>
-    <row r="9" spans="1:11" ht="30">
+    <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>22</v>
       </c>
@@ -1887,7 +1901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30">
+    <row r="10" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>24</v>
       </c>
@@ -1923,7 +1937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -1957,7 +1971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30">
+    <row r="12" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
@@ -2003,14 +2017,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
@@ -2018,7 +2032,7 @@
     <col min="4" max="4" width="136.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -2032,7 +2046,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2047,7 +2061,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2062,7 +2076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2076,7 +2090,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2090,7 +2104,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2105,7 +2119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2119,7 +2133,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -2133,7 +2147,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -2147,7 +2161,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>20</v>
       </c>
@@ -2161,7 +2175,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>20</v>
       </c>
@@ -2175,7 +2189,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -2189,7 +2203,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>31</v>
       </c>
@@ -2203,7 +2217,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -2217,7 +2231,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
@@ -2231,7 +2245,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
         <v>32</v>
       </c>
@@ -2245,7 +2259,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
         <v>32</v>
       </c>
@@ -2259,7 +2273,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
         <v>32</v>
       </c>
@@ -2273,7 +2287,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
         <v>33</v>
       </c>
@@ -2287,7 +2301,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
         <v>33</v>
       </c>
@@ -2301,7 +2315,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
         <v>33</v>
       </c>
@@ -2315,7 +2329,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
         <v>34</v>
       </c>
@@ -2329,7 +2343,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
         <v>34</v>
       </c>
@@ -2343,7 +2357,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
         <v>34</v>
       </c>
@@ -2357,7 +2371,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>22</v>
       </c>
@@ -2371,7 +2385,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>22</v>
       </c>
@@ -2385,7 +2399,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -2399,7 +2413,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2413,7 +2427,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2427,7 +2441,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2453,21 +2467,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>72</v>
       </c>
@@ -2478,7 +2492,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -2489,7 +2503,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
@@ -2500,7 +2514,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
@@ -2511,7 +2525,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>13</v>
       </c>
@@ -2522,7 +2536,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>52</v>
       </c>
@@ -2533,7 +2547,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2544,7 +2558,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
@@ -2555,7 +2569,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>22</v>
       </c>
@@ -2566,7 +2580,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>24</v>
       </c>
@@ -2577,7 +2591,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -2588,7 +2602,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
@@ -2611,21 +2625,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>72</v>
       </c>
@@ -2636,7 +2650,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -2647,7 +2661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
@@ -2658,7 +2672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
@@ -2669,7 +2683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>13</v>
       </c>
@@ -2680,7 +2694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>52</v>
       </c>
@@ -2691,7 +2705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2702,7 +2716,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
@@ -2713,7 +2727,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>22</v>
       </c>
@@ -2724,7 +2738,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>24</v>
       </c>
@@ -2735,7 +2749,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -2746,7 +2760,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
@@ -2769,14 +2783,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -2784,7 +2798,7 @@
     <col min="4" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
         <v>73</v>
       </c>
@@ -2801,7 +2815,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2809,7 +2823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2817,7 +2831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2825,7 +2839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2833,7 +2847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2841,7 +2855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2852,7 +2866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2860,7 +2874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2868,7 +2882,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2876,7 +2890,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2884,7 +2898,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -2898,7 +2912,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -2912,7 +2926,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -2926,7 +2940,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -2939,11 +2953,8 @@
       <c r="D15" t="s">
         <v>28</v>
       </c>
-      <c r="E15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -2960,7 +2971,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -2977,7 +2988,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>84</v>
       </c>

</xml_diff>